<commit_message>
Feladat módosítás bugfix. Feladatok feltöltése
</commit_message>
<xml_diff>
--- a/Feladatok/TortenelemFeladatok.xlsx
+++ b/Feladatok/TortenelemFeladatok.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernát Olivér\Desktop\projektFeladat\Admin\Feladatok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog gyak\Gyakorlás\14_D - Hazi\Erettsegizzunk\Admin\Feladatok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4648D3-005B-4921-A10F-CD4A6C1C2610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{97C2F95F-C29F-4DCA-A979-355909D69C2E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,9 +64,6 @@
     <t>PicName</t>
   </si>
   <si>
-    <t>A feladat a kereszténység főbb tanításaihoz kapcsolódik. Oldja meg a feladatokat a forrás és ismeretei segítségével!</t>
-  </si>
-  <si>
     <t>„Hallottátok, hogy a régiek ezt a parancsot kapták: Ne ölj! Aki öl, állítsák a törvényszék elé. Én pedig azt mondom nektek: Már azt is állítsák a törvényszék elé, aki haragot tart embertársával. […] Hallottátok a parancsot: Szemet szemért és fogat fogért. Én pedig azt mondom nektek, ne álljatok ellent a gonosznak. Aki megüti a jobb arcodat, annak tartsd oda a másikat is! […] Hallottátok a parancsot: Szeresd felebarátodat, és gyűlöld ellenségedet! Én pedig azt mondom nektek: Szeressétek ellenségeiteket, és imádkozzatok üldözőitekért! Így lesztek fiai mennyei Atyátoknak, aki fölkelti napját jókra is, gonoszokra is, esőt ad igazaknak is, bűnösöknek is. Ha csupán azokat szeretitek, akik szeretnek benneteket, mi lesz a jutalmatok?” (Részletek Jézus hegyi beszédéből, Máté evangéliuma)</t>
   </si>
   <si>
@@ -89,9 +85,6 @@
     <t>Mohamed</t>
   </si>
   <si>
-    <t xml:space="preserve">A feladat az iszlám vallással kapcsolatos. Oldja meg a feladatokat a források és ismeretei segítségével! Nevezze meg azt a személyt, akit a szerző – egyes szám első személyt használva – idéz! </t>
-  </si>
-  <si>
     <t>A;B;C</t>
   </si>
   <si>
@@ -101,24 +94,12 @@
     <t>0;1;0</t>
   </si>
   <si>
-    <t xml:space="preserve">A feladat az iszlám vallással kapcsolatos. Oldja meg a feladatokat a források és ismeretei segítségével!  Nevezze meg azt az írásművet, amely ezen esemény következtében született meg! </t>
-  </si>
-  <si>
-    <t>A feladat az iszlám vallással kapcsolatos. Oldja meg a feladatokat a források és ismeretei segítségével!  Jelölje ki a forrásban leírt eseményt ábrázoló kép betűjelét! Egyetlen betűjelet jelöljön ki!</t>
-  </si>
-  <si>
     <t>Korán</t>
   </si>
   <si>
-    <t xml:space="preserve">A feladat az iszlám vallással kapcsolatos. Oldja meg a feladatokat a források és ismeretei segítségével!  A vallás megszületésének mely mozzanatát mutatja be a szöveges forrás? Jelölje ki az egyetlen helyes állítást! </t>
-  </si>
-  <si>
     <t>1;0;0</t>
   </si>
   <si>
-    <t xml:space="preserve">A feladat az angol alkotmányos monarchia történetéhez kapcsolódik. Válassza ki a forrás betűvel jelölt részletei közül azokat, amelyek az igazságszolgáltatást szabályozzák, illetve azokat, amelyek a végrehajtó hatalom ellenőrzéséről szólnak! Írja a betűjeleket a táblázat megfelelő mezőibe! </t>
-  </si>
-  <si>
     <t xml:space="preserve">1. A mű főszereplője próféta lett.;2. Kezdetét vette az iszlám időszámítás.;3. A mű főszereplője mennybe ment. </t>
   </si>
   <si>
@@ -143,18 +124,12 @@
     <t>0;0;1</t>
   </si>
   <si>
-    <t>A feladat az 1848-as forradalommal kapcsolatos.Mire utal az idézett beszéd b) betűvel jelzett, aláhúzott része? Jelölje ki az egyetlen helyes válasz sorszámát!</t>
-  </si>
-  <si>
     <t xml:space="preserve">A feladat az 1848-as forradalommal kapcsolatos.Melyik állítás támasztja alá az idézett beszéd a) betűvel jelzett, aláhúzott részét? Jelölje ki az egyetlen helyes állítás sorszámát! </t>
   </si>
   <si>
     <t xml:space="preserve"> jobbágyfelszabadítás;örökváltság;úrbéri viszonyok megszüntetése;közteherviselés; törvény előtti egyenlőség ; jogkiterjesztés</t>
   </si>
   <si>
-    <t>1;1;1;1;1;1;1</t>
-  </si>
-  <si>
     <t>Pozsony</t>
   </si>
   <si>
@@ -167,9 +142,6 @@
     <t>„A költségvetésnek egészséges és tartós alapokon nyugvó egyensúlya a jelen jegyzőkönyv értelmében csak akkor tekinthető elértnek, ha […] lehetséges lesz a kiadások sorába felvenni a kölcsönszolgálat [a hitel] terheit és a trianoni szerződésből folyó terheket. […] A programnak ki kell zárnia [más] kölcsönök igénybevételét, […] és a bankjegyinfláció mindennemű igénybevétele ki lesz zárva. […] Magyarország hozzájárul ahhoz, hogy a Nemzetek Szövetségének Tanácsa főbiztost nevezzen ki. […] A főbiztosnak hivatása, hogy felügyeljen a reformprogram teljes végrehajtására, és […] biztosítsa […], hogy a költségvetés egyensúlya […] eléressék. […] A magyar kormány a […] kölcsön biztosítékául leköti a vámjövedék, a cukoradó és a dohányjövedék nyers bevételét, valamint a sójövedék tiszta bevételét.” (A népszövetségi kölcsönről aláírt jegyzőkönyv, 1924)</t>
   </si>
   <si>
-    <t>A feladat a Horthy-korszakkal kapcsolatos. Karikázza be a jegyzőkönyv idézett részlete alapján igazolható két helyes állítás sorszámát!</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. A pénzügyi stabilitás megteremtéséhez a nagyszabású földreform is hozzájárult.;2. A kormány ígéretet tett arra, hogy bizonyos jövedelmeket a hitel törlesztésére fordít.;3. A befolyt összeget a hadsereg fejlesztésére fordították.;4. A költségvetési kiadásoknál figyelembe kellett venni a hiteltörlesztést is.;5. A költségvetési egyensúlyt újabb hitelek felvétele is segíthette. </t>
   </si>
   <si>
@@ -191,9 +163,6 @@
     <t>A feladat a Horthy-korszakkal kapcsolatos. Mit ír körül a forrás aláhúzott része? Nevezze meg szakkifejezéssel!</t>
   </si>
   <si>
-    <t>A feladat a holokauszt történetéhez kapcsolódik. Döntse el, melyik forrásrészletekben leírtakra vonatkoznak a táblázatban szereplő állítások! Írja a forrásrészlet betűjelét a táblázat megfelelő mezőjébe!</t>
-  </si>
-  <si>
     <t>A) „A Szovjetunió megtámadása után [1941-ben] Románia hozzákezdett saját végleges megoldási programjának végrehajtásához. A román hadsereg és csendőrség egységei, […] súlyos tömeggyilkosságokban vettek részt. Antonescu marsall [a Romániát vezető diktátor] parancsára majdnem 150 000 zsidót deportáltak […] Transznisztriába [a Szovjetuniótól meghódított és Romániához csatolt területre].” \nB) „A horvátok már akkor »megoldották« a maguk zsidókérdésének jó részét […], amikor függetlenségük elnyerése után [értsd: a Jugoszláviától való elszakadás után] nyomban felléptek a szerb és cigány [és zsidó] lakosság ellen. 1941 októberében, majd 1942 májusában is a horvátok azt kérelmezték a német Külügyminisztériumnál, hogy a németek deportálják a megmaradt zsidókat [és az meg is történt].” \nC) „A szlovákok […] teljesítették a zsidósággal kapcsolatos német kéréseket. Szlovákia zsidósága elsőként esett áldozatául a [németországi] wannsee-i konferencián elhatározott végleges megoldásnak. 1942 februárjának elején Szlovákia vállalta, hogy »20 000 fiatal, erős szlovák zsidót« ad át a németeknek. […] A zsidó családok együttmaradása érdekében az átadott férfiak családtagjait is deportálásra javasolták.”</t>
   </si>
   <si>
@@ -215,20 +184,50 @@
     <t>_</t>
   </si>
   <si>
-    <t xml:space="preserve">A feladat az 1848-as forradalommal kapcsolatos.  A forrás szerzője a jellemzően a birtokos nemesek közé tartozó követtársaihoz beszélt. Melyik intézkedés volt a legjelentősebb oka annak a változásnak, amelyre az idézett beszéd c) betűvel jelzett, aláhúzott része utal? Nevezze meg szakkifejezéssel! </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A feladat az 1848-as forradalommal kapcsolatos. Mely városban hangzott el az idézett beszéd? Nevezze meg a várost! Melyik intézkedés volt a legjelentősebb oka annak a változásnak, amelyre az idézett beszéd c) betűvel jelzett, aláhúzott része utal? Nevezze meg szakkifejezéssel! </t>
-  </si>
-  <si>
     <t>A feladat a polgári állam jellemzőivel kapcsolatos. Rendelje a következő forrásokat a a szövegdobozokban szereplő állítsok közül ahhoz, amelyet közvetlenül alátámasztanak! Írja a források betűjelét a táblázat megfelelő mezőjébe! Egy mezőbe egy betűjelet írjon! Egy betűjel kétszer is szerepelhet.</t>
+  </si>
+  <si>
+    <t>A feladat a kereszténység főbb tanításaihoz kapcsolódik. Mely vallás követőire vonatkozik az idézett forrásban aláhúzott szó?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A feladat az iszlám vallással kapcsolatos. Nevezze meg azt a személyt, akit a szerző – egyes szám első személyt használva – idéz! </t>
+  </si>
+  <si>
+    <t>A feladat az iszlám vallással kapcsolatos. Jelölje ki a forrásban leírt eseményt ábrázoló kép betűjelét! Egyetlen betűjelet jelöljön ki!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A feladat az iszlám vallással kapcsolatos. Nevezze meg azt az írásművet, amely ezen esemény következtében született meg! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A feladat az iszlám vallással kapcsolatos. A vallás megszületésének mely mozzanatát mutatja be a szöveges forrás? Jelölje ki az egyetlen helyes állítást! </t>
+  </si>
+  <si>
+    <t>A feladat az 1848-as forradalommal kapcsolatos. Mely városban hangzott el az idézett beszéd? Nevezze meg a várost!</t>
+  </si>
+  <si>
+    <t>1;1;1;1;1;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A feladat az angol alkotmányos monarchia történetéhez kapcsolódik. Válassza ki a forrás betűvel jelölt részletei közül azokat, amelyek az igazságszolgáltatást szabályozzák, illetve azokat, amelyek a végrehajtó hatalom ellenőrzéséről szólnak! Írja a betűjeleket a megfelelő mezőkbe! </t>
+  </si>
+  <si>
+    <t>A feladat az 1848-as forradalommal kapcsolatos. Mire utal az idézett beszéd b) betűvel jelzett, aláhúzott része? Jelölje ki az egyetlen helyes válasz sorszámát!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A feladat az 1848-as forradalommal kapcsolatos. A forrás szerzője a jellemzően a birtokos nemesek közé tartozó követtársaihoz beszélt. Melyik intézkedés volt a legjelentősebb oka annak a változásnak, amelyre az idézett beszéd c) betűvel jelzett, aláhúzott része utal? Nevezze meg szakkifejezéssel! </t>
+  </si>
+  <si>
+    <t>A feladat a Horthy-korszakkal kapcsolatos. Jelölje ki a jegyzőkönyv idézett részlete alapján igazolható két helyes állítás sorszámát!</t>
+  </si>
+  <si>
+    <t>A feladat a holokauszt történetéhez kapcsolódik. Döntse el, melyik forrásrészletekben leírtakra vonatkoznak a táblázatban szereplő állítások! Írja a forrásrészlet betűjelét a megfelelő mezőbe!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,21 +603,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BABE57F-5A5E-496E-BC40-FFD88534DEDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="64.33203125" customWidth="1"/>
-    <col min="2" max="2" width="82.6640625" customWidth="1"/>
-    <col min="3" max="3" width="34.21875" customWidth="1"/>
+    <col min="1" max="1" width="49.8984375" customWidth="1"/>
+    <col min="2" max="2" width="82.69921875" customWidth="1"/>
+    <col min="3" max="3" width="34.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,18 +646,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -673,18 +672,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -699,15 +698,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -724,22 +723,19 @@
       <c r="H4">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -753,16 +749,19 @@
       <c r="H5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -780,18 +779,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -806,18 +805,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -832,18 +831,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -858,18 +857,18 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -884,18 +883,18 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -910,15 +909,15 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -936,18 +935,18 @@
         <v>12.13</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -962,18 +961,18 @@
         <v>14.15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -988,15 +987,15 @@
         <v>17.18</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1014,15 +1013,15 @@
         <v>17.18</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1040,18 +1039,18 @@
         <v>17.18</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1066,18 +1065,18 @@
         <v>16.18</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -1092,7 +1091,7 @@
         <v>18.190000000000001</v>
       </c>
       <c r="I18" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>